<commit_message>
Vez metal print head with Goliath short
</commit_message>
<xml_diff>
--- a/bom/BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC.xlsx
+++ b/bom/BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC.xlsx
@@ -736,16 +736,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -760,7 +751,16 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2674,8 +2674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2697,90 +2697,90 @@
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="29" t="str">
+      <c r="E1" s="21" t="str">
         <f>HYPERLINK("https://a360.co/47wpYBq","LINK TO CAD")</f>
         <v>LINK TO CAD</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="27"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="21" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
     </row>
     <row r="3" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="21" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="21" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="24" t="s">
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="21" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="24" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
Prerequisit for ZR2.6 High Reach added to Goliath Short
</commit_message>
<xml_diff>
--- a/bom/BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC.xlsx
+++ b/bom/BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e8bf86f88c49aa82/Documents/GitHub/HevORT/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{50ADFD7E-3A6B-42DB-95C4-F3352E1663F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F65C82D-17E6-4DB3-BDC5-576B94D1EFB7}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{50ADFD7E-3A6B-42DB-95C4-F3352E1663F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{222AB613-2A3B-42FB-B53C-3D9534F71EF7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -294,9 +294,6 @@
     <t>For Goliath Short installation.  (HextrudORT is the Heat sink)</t>
   </si>
   <si>
-    <t>HDx_VZ Metal Print Head Watercooled Goliath Short</t>
-  </si>
-  <si>
     <t>Cooling duct Sliding mount</t>
   </si>
   <si>
@@ -325,9 +322,6 @@
   </si>
   <si>
     <t>No official config yet</t>
-  </si>
-  <si>
-    <t>To come</t>
   </si>
   <si>
     <t>Set #13 does not include any Heat Sink.  
@@ -371,12 +365,45 @@
   <si>
     <t>https://github.com/MirageC79/HevORT/tree/master/files/STL/PrintHead/VezMetalPrintHead_HDx</t>
   </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_DkWpMEx</t>
+  </si>
+  <si>
+    <t>Heat break required for 
+Goliath Short to fit in 
+VZ HextrudORT WaterCooled</t>
+  </si>
+  <si>
+    <t>https://discord.com/channels/790612368056647682/819621988409802823/1142211491475505292</t>
+  </si>
+  <si>
+    <t>https://docs.hevort.com/#/pages/component-selection?id=a-water-cooling-bay</t>
+  </si>
+  <si>
+    <t>ZR2.6 High Reach Mod (Goliath Short, is very short ;) )</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">HDx_VZ Metal Print Head Watercooled Goliath </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF76933C"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>SHORT</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,13 +566,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <i/>
       <sz val="14"/>
       <name val="Calibri"/>
@@ -557,6 +577,35 @@
       <u/>
       <sz val="28"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF76933C"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -674,7 +723,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -736,7 +785,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -754,13 +803,19 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1132,13 +1187,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1514538</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1638300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1176,13 +1231,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1220,13 +1275,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1264,13 +1319,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1308,13 +1363,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1352,13 +1407,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1396,13 +1451,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1440,13 +1495,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1484,13 +1539,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1528,13 +1583,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1572,13 +1627,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1616,13 +1671,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1660,13 +1715,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1704,13 +1759,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1748,13 +1803,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149226</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>168275</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1324916</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>1289050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1797,7 +1852,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1075765</xdr:colOff>
+      <xdr:colOff>1082115</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3999965</xdr:rowOff>
     </xdr:to>
@@ -1836,13 +1891,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>226391</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>187739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1258956</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1220304</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1880,14 +1935,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>77304</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1414865</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1308652</xdr:rowOff>
+      <xdr:colOff>1424390</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1311827</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1924,14 +1979,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1498600</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>254000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2520950</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1340289</xdr:rowOff>
+      <xdr:colOff>2530475</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1349814</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1968,13 +2023,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2711451</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>285751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3727451</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:colOff>3730626</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1317538</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2012,14 +2067,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1803400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1195328</xdr:rowOff>
+      <xdr:colOff>1806575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1198503</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2056,13 +2111,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2254251</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3695700</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1234021</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2100,13 +2155,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1670050</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:colOff>1673225</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1236832</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2144,13 +2199,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2279650</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3587749</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:colOff>3597274</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>1239993</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2188,14 +2243,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2543972</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3919011</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>1644650</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15629</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1654175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2232,13 +2287,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1123951</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>927101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>2470151</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:colOff>2473326</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1617211</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2276,13 +2331,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2666999</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>59920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3922058</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2801</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>1313555</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2320,14 +2375,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>2547471</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>3806407</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1344706</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1347881</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2364,8 +2419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8B7DE9-2806-43F2-BF40-0CB9E0E8C833}" name="Table1" displayName="Table1" ref="A6:K23" totalsRowShown="0">
-  <autoFilter ref="A6:K23" xr:uid="{FF8B7DE9-2806-43F2-BF40-0CB9E0E8C833}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8B7DE9-2806-43F2-BF40-0CB9E0E8C833}" name="Table1" displayName="Table1" ref="A7:K24" totalsRowShown="0">
+  <autoFilter ref="A7:K24" xr:uid="{FF8B7DE9-2806-43F2-BF40-0CB9E0E8C833}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{23AD65AB-EB34-4EF2-A78F-F538F4B7C05F}" name="SubAssy" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{99CC5EA5-BAB8-4C38-91EF-937575D0F8EF}" name="Category" dataDxfId="9">
@@ -2672,27 +2727,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7265625" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" customWidth="1"/>
-    <col min="5" max="5" width="37.81640625" customWidth="1"/>
-    <col min="6" max="6" width="32.1796875" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" customWidth="1"/>
-    <col min="9" max="9" width="57.54296875" customWidth="1"/>
-    <col min="10" max="10" width="19.7265625" customWidth="1"/>
-    <col min="11" max="11" width="32.90625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="57.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="11" customFormat="1" ht="336.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="11" customFormat="1" ht="336.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -2712,254 +2767,243 @@
       </c>
       <c r="K1" s="24"/>
     </row>
-    <row r="2" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="I2" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
     </row>
-    <row r="3" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
-      <c r="I3" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="I3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
     </row>
-    <row r="4" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="26" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
       <c r="I4" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
+        <v>88</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
     </row>
-    <row r="5" spans="1:11" s="11" customFormat="1" ht="38" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
       <c r="H5" s="26"/>
       <c r="I5" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+        <v>89</v>
+      </c>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
     </row>
-    <row r="6" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+    </row>
+    <row r="7" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K7" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="143.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="13" t="str">
+    <row r="8" spans="1:11" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H8" s="13">
         <v>1</v>
       </c>
-      <c r="I7" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="17" t="s">
+      <c r="I8" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="18" t="s">
-        <v>73</v>
+      <c r="K8" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="13" t="str">
+    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>*</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="13" t="str">
-        <f>Table1[[#This Row],[Make/Buy]]</f>
-        <v>Buy</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="15"/>
+        <v>71</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="G9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="13">
-        <v>1</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>83</v>
+        <v>44</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="K9" s="18"/>
     </row>
-    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B10" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>69</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H10" s="13">
         <v>1</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="20" t="s">
+        <v>81</v>
+      </c>
       <c r="J10" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="K10" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B11" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="15" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>9</v>
@@ -2967,28 +3011,34 @@
       <c r="H11" s="13">
         <v>1</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="J11" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="K11" s="18"/>
+        <v>82</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B12" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="15"/>
+        <v>27</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>70</v>
+      </c>
       <c r="G12" s="13" t="s">
         <v>9</v>
       </c>
@@ -2997,26 +3047,26 @@
       </c>
       <c r="I12" s="16"/>
       <c r="J12" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B13" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="13" t="s">
@@ -3025,171 +3075,167 @@
       <c r="H13" s="13">
         <v>1</v>
       </c>
-      <c r="I13" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="I13" s="16"/>
       <c r="J13" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K13" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B14" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="15" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="13">
-        <v>11</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B15" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H15" s="13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I15" s="16"/>
       <c r="J15" s="17"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B16" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I16" s="16"/>
       <c r="J16" s="17"/>
       <c r="K16" s="18"/>
     </row>
-    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B17" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="13">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="17"/>
       <c r="K17" s="18"/>
     </row>
-    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B18" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>48</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="F18" s="15"/>
       <c r="G18" s="13" t="s">
         <v>9</v>
       </c>
       <c r="H18" s="13">
-        <v>1</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>50</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="18"/>
     </row>
-    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B19" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Buy</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>9</v>
@@ -3197,58 +3243,62 @@
       <c r="H19" s="13">
         <v>1</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="J19" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B20" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
-        <v>Make</v>
+        <v>Buy</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="G20" s="13" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H20" s="13">
         <v>1</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>87</v>
+        <v>41</v>
+      </c>
+      <c r="K20" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B21" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Make</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="15" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="13" t="s">
@@ -3257,30 +3307,28 @@
       <c r="H21" s="13">
         <v>1</v>
       </c>
-      <c r="I21" s="16" t="s">
-        <v>53</v>
-      </c>
+      <c r="I21" s="16"/>
       <c r="J21" s="17" t="s">
         <v>54</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B22" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Make</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="15" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="13" t="s">
@@ -3290,29 +3338,29 @@
         <v>1</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J22" s="17" t="s">
         <v>54</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B23" s="13" t="str">
         <f>Table1[[#This Row],[Make/Buy]]</f>
         <v>Make</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="15"/>
       <c r="G23" s="13" t="s">
@@ -3321,48 +3369,89 @@
       <c r="H23" s="13">
         <v>1</v>
       </c>
-      <c r="I23" s="16"/>
+      <c r="I23" s="16" t="s">
+        <v>55</v>
+      </c>
       <c r="J23" s="17" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="13" t="str">
+        <f>Table1[[#This Row],[Make/Buy]]</f>
+        <v>Make</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A2:D5"/>
+    <mergeCell ref="A2:D6"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
     <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="I3:K3"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="E4:H4"/>
     <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K18" r:id="rId1" xr:uid="{5915F819-8D0D-4096-AB64-ACDEC0950CFD}"/>
-    <hyperlink ref="K19" r:id="rId2" xr:uid="{63A27367-B8F4-4816-91AA-B9EC57B3D733}"/>
-    <hyperlink ref="K13" r:id="rId3" xr:uid="{FB370755-8450-4908-994F-C3C55521888F}"/>
+    <hyperlink ref="K19" r:id="rId1" xr:uid="{5915F819-8D0D-4096-AB64-ACDEC0950CFD}"/>
+    <hyperlink ref="K20" r:id="rId2" xr:uid="{63A27367-B8F4-4816-91AA-B9EC57B3D733}"/>
+    <hyperlink ref="K14" r:id="rId3" xr:uid="{FB370755-8450-4908-994F-C3C55521888F}"/>
     <hyperlink ref="I2" r:id="rId4" location="/pages/component-selection?id=_2-xy-gantry" xr:uid="{1B958F30-2683-4626-A2AC-C7C6A5B7EC00}"/>
     <hyperlink ref="I3" r:id="rId5" location="/pages/component-selection?id=x-axis-options" xr:uid="{DB3F8C6B-2862-42E7-85D0-BB9B22ADC016}"/>
-    <hyperlink ref="K20" r:id="rId6" xr:uid="{DE84B033-617B-45C9-A0FE-3BB7620C3F32}"/>
-    <hyperlink ref="K21" r:id="rId7" xr:uid="{FB6A82D8-D5AE-437C-9107-07DB72480C5A}"/>
-    <hyperlink ref="K22" r:id="rId8" xr:uid="{A6EFD336-5FD9-474E-8E64-CDE3C7E96678}"/>
-    <hyperlink ref="K23" r:id="rId9" xr:uid="{2077A0AB-7477-48B0-A2AC-F66676C89C70}"/>
+    <hyperlink ref="K21" r:id="rId6" xr:uid="{DE84B033-617B-45C9-A0FE-3BB7620C3F32}"/>
+    <hyperlink ref="K22" r:id="rId7" xr:uid="{FB6A82D8-D5AE-437C-9107-07DB72480C5A}"/>
+    <hyperlink ref="K23" r:id="rId8" xr:uid="{A6EFD336-5FD9-474E-8E64-CDE3C7E96678}"/>
+    <hyperlink ref="K24" r:id="rId9" xr:uid="{2077A0AB-7477-48B0-A2AC-F66676C89C70}"/>
+    <hyperlink ref="K8" r:id="rId10" xr:uid="{91FBA0FA-2181-46C3-930A-B1CF42A137D8}"/>
+    <hyperlink ref="K10" r:id="rId11" xr:uid="{A52635FB-5DB1-4D1B-A035-0662F9ADB73A}"/>
+    <hyperlink ref="K13" r:id="rId12" xr:uid="{D6E831ED-08EC-4A85-8B5B-7C48E66B4940}"/>
+    <hyperlink ref="K12" r:id="rId13" xr:uid="{0271D5E1-D71D-4F6C-9123-B32F4D965123}"/>
+    <hyperlink ref="K11" r:id="rId14" xr:uid="{574B6A18-506B-4A6F-A152-6350E6514B2C}"/>
+    <hyperlink ref="I4" r:id="rId15" xr:uid="{38B6B54C-3CB4-4213-A7C7-40F3F6D682D7}"/>
+    <hyperlink ref="I5" r:id="rId16" location="/pages/component-selection?id=a-water-cooling-bay" xr:uid="{9D55C7EC-ED9C-4E6F-9F0A-56C2CE795472}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId17"/>
+  <drawing r:id="rId18"/>
   <webPublishItems count="1">
     <webPublishItem id="8106" divId="BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC_8106" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_VezMetalPrintHead_GoliathShort_VZHextrudORT_WC.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>